<commit_message>
Ui updates + minor fixes
</commit_message>
<xml_diff>
--- a/data/figure_classification_final.xlsx
+++ b/data/figure_classification_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acrisan/Projects/gevit_gallery_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{FDBF190C-1BB7-5F45-A5B2-D1C307C7867B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D916D6FE-DC31-1044-BECB-19268955F1BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="-15480" windowWidth="26300" windowHeight="15920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2780" yWindow="-18620" windowWidth="26300" windowHeight="15920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure Analysis with Classifica" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8612" uniqueCount="1825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8612" uniqueCount="1823">
   <si>
     <t>PMID</t>
   </si>
@@ -4921,9 +4921,6 @@
     <t>line[bracket];text</t>
   </si>
   <si>
-    <t>text;line[shape;colour];text[colour]</t>
-  </si>
-  <si>
     <t>line[texture];text[colour]</t>
   </si>
   <si>
@@ -5284,9 +5281,6 @@
     <t>Table;Distribution Chart;Line Chart</t>
   </si>
   <si>
-    <t>Image;Stream Plot;Category Stripe</t>
-  </si>
-  <si>
     <t>Tree;Distribution Chart;Geographic Map;Node-link</t>
   </si>
   <si>
@@ -5413,9 +5407,6 @@
     <t>NA;NA;Alignment</t>
   </si>
   <si>
-    <t>NA;Phylgenetic Tree - Rooted</t>
-  </si>
-  <si>
     <t>Genomic Map;Timeline</t>
   </si>
   <si>
@@ -5507,6 +5498,9 @@
   </si>
   <si>
     <t>containment mark;glyph[pie chart [size] ]</t>
+  </si>
+  <si>
+    <t>Image;Flow Diagram;Category Stripe</t>
   </si>
 </sst>
 </file>
@@ -5956,9 +5950,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M856"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F157" sqref="F157"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A713" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C733" sqref="C733"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6417,7 +6411,7 @@
         <v>930</v>
       </c>
       <c r="G13" t="s">
-        <v>1799</v>
+        <v>1796</v>
       </c>
       <c r="H13" t="s">
         <v>930</v>
@@ -7259,7 +7253,7 @@
         <v>16208372</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>955</v>
@@ -8297,7 +8291,7 @@
         <v>940</v>
       </c>
       <c r="F68" t="s">
-        <v>1811</v>
+        <v>1808</v>
       </c>
       <c r="G68" t="s">
         <v>930</v>
@@ -8399,7 +8393,7 @@
         <v>969</v>
       </c>
       <c r="F71" t="s">
-        <v>1812</v>
+        <v>1809</v>
       </c>
       <c r="G71" t="s">
         <v>930</v>
@@ -8717,7 +8711,7 @@
         <v>940</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>1813</v>
+        <v>1810</v>
       </c>
       <c r="G80" s="3" t="s">
         <v>930</v>
@@ -9258,7 +9252,7 @@
         <v>940</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>1799</v>
+        <v>1796</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>930</v>
@@ -9295,7 +9289,7 @@
         <v>940</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>1814</v>
+        <v>1811</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>930</v>
@@ -9332,7 +9326,7 @@
         <v>940</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>1799</v>
+        <v>1796</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>930</v>
@@ -9788,7 +9782,7 @@
         <v>930</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="L109" s="1" t="s">
         <v>426</v>
@@ -9802,7 +9796,7 @@
         <v>20375036</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>1616</v>
@@ -9826,7 +9820,7 @@
         <v>930</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="L110" s="1" t="s">
         <v>426</v>
@@ -10178,7 +10172,7 @@
         <v>1015</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>1815</v>
+        <v>1812</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>930</v>
@@ -10215,7 +10209,7 @@
         <v>1015</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>1815</v>
+        <v>1812</v>
       </c>
       <c r="G121" s="3" t="s">
         <v>930</v>
@@ -10332,7 +10326,7 @@
         <v>1102</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>1823</v>
+        <v>1820</v>
       </c>
       <c r="I124" s="3" t="s">
         <v>1103</v>
@@ -10394,7 +10388,7 @@
         <v>1079</v>
       </c>
       <c r="D126" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>967</v>
@@ -10885,7 +10879,7 @@
         <v>993</v>
       </c>
       <c r="F139" t="s">
-        <v>1808</v>
+        <v>1805</v>
       </c>
       <c r="G139" t="s">
         <v>930</v>
@@ -11498,41 +11492,41 @@
         <v>935</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A157">
+    <row r="157" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="11">
         <v>21984923</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C157" s="11" t="s">
         <v>822</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D157" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E157" s="11" t="s">
         <v>967</v>
       </c>
-      <c r="F157" t="s">
-        <v>1824</v>
-      </c>
-      <c r="G157" t="s">
+      <c r="F157" s="11" t="s">
+        <v>1821</v>
+      </c>
+      <c r="G157" s="11" t="s">
         <v>1004</v>
       </c>
-      <c r="H157" t="s">
+      <c r="H157" s="11" t="s">
         <v>994</v>
       </c>
-      <c r="I157" t="s">
+      <c r="I157" s="11" t="s">
         <v>1128</v>
       </c>
-      <c r="J157" t="s">
+      <c r="J157" s="11" t="s">
         <v>1406</v>
       </c>
-      <c r="L157" t="s">
+      <c r="L157" s="11" t="s">
         <v>1127</v>
       </c>
-      <c r="M157" t="s">
+      <c r="M157" s="11" t="s">
         <v>935</v>
       </c>
     </row>
@@ -11693,7 +11687,7 @@
         <v>1015</v>
       </c>
       <c r="F162" t="s">
-        <v>1816</v>
+        <v>1813</v>
       </c>
       <c r="G162" t="s">
         <v>930</v>
@@ -11719,7 +11713,7 @@
         <v>236</v>
       </c>
       <c r="C163" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="D163" t="s">
         <v>1529</v>
@@ -11816,38 +11810,38 @@
         <v>935</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A166">
+    <row r="166" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="11">
         <v>22084315</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C166" s="11" t="s">
         <v>955</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="11" t="s">
         <v>813</v>
       </c>
-      <c r="E166" t="s">
-        <v>940</v>
-      </c>
-      <c r="F166" t="s">
-        <v>1629</v>
-      </c>
-      <c r="G166" t="s">
-        <v>930</v>
-      </c>
-      <c r="H166" t="s">
-        <v>930</v>
-      </c>
-      <c r="I166" t="s">
+      <c r="E166" s="11" t="s">
+        <v>940</v>
+      </c>
+      <c r="F166" s="11" t="s">
+        <v>1604</v>
+      </c>
+      <c r="G166" s="11" t="s">
+        <v>930</v>
+      </c>
+      <c r="H166" s="11" t="s">
+        <v>930</v>
+      </c>
+      <c r="I166" s="11" t="s">
         <v>1134</v>
       </c>
-      <c r="L166" t="s">
-        <v>930</v>
-      </c>
-      <c r="M166" t="s">
+      <c r="L166" s="11" t="s">
+        <v>930</v>
+      </c>
+      <c r="M166" s="11" t="s">
         <v>935</v>
       </c>
     </row>
@@ -11941,7 +11935,7 @@
         <v>1071</v>
       </c>
       <c r="G169" s="3" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="H169" s="3" t="s">
         <v>930</v>
@@ -12142,7 +12136,7 @@
         <v>1111</v>
       </c>
       <c r="D175" t="s">
-        <v>1776</v>
+        <v>1774</v>
       </c>
       <c r="E175" t="s">
         <v>1256</v>
@@ -12393,7 +12387,7 @@
         <v>940</v>
       </c>
       <c r="F182" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="G182" t="s">
         <v>930</v>
@@ -12472,13 +12466,13 @@
         <v>930</v>
       </c>
       <c r="I184" s="3" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="J184" s="3" t="s">
         <v>1404</v>
       </c>
       <c r="K184" s="3" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="L184" s="3" t="s">
         <v>930</v>
@@ -12740,10 +12734,10 @@
         <v>463</v>
       </c>
       <c r="C192" s="3" t="s">
+        <v>1633</v>
+      </c>
+      <c r="D192" s="3" t="s">
         <v>1634</v>
-      </c>
-      <c r="D192" s="3" t="s">
-        <v>1635</v>
       </c>
       <c r="E192" s="3" t="s">
         <v>1301</v>
@@ -12950,10 +12944,10 @@
         <v>839</v>
       </c>
       <c r="C198" s="3" t="s">
+        <v>1739</v>
+      </c>
+      <c r="D198" s="3" t="s">
         <v>1740</v>
-      </c>
-      <c r="D198" s="3" t="s">
-        <v>1741</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>1303</v>
@@ -12971,7 +12965,7 @@
         <v>930</v>
       </c>
       <c r="K198" s="3" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="M198" s="3" t="s">
         <v>935</v>
@@ -12985,16 +12979,16 @@
         <v>840</v>
       </c>
       <c r="C199" s="3" t="s">
+        <v>1635</v>
+      </c>
+      <c r="D199" s="3" t="s">
         <v>1636</v>
-      </c>
-      <c r="D199" s="3" t="s">
-        <v>1637</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>1267</v>
       </c>
       <c r="F199" s="3" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="G199" s="3" t="s">
         <v>986</v>
@@ -13006,7 +13000,7 @@
         <v>930</v>
       </c>
       <c r="K199" s="3" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="L199" s="3" t="s">
         <v>930</v>
@@ -13023,10 +13017,10 @@
         <v>841</v>
       </c>
       <c r="C200" s="3" t="s">
+        <v>1640</v>
+      </c>
+      <c r="D200" s="3" t="s">
         <v>1641</v>
-      </c>
-      <c r="D200" s="3" t="s">
-        <v>1642</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>967</v>
@@ -13038,13 +13032,13 @@
         <v>1213</v>
       </c>
       <c r="H200" s="3" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="I200" s="3" t="s">
         <v>930</v>
       </c>
       <c r="K200" s="3" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="L200" s="3" t="s">
         <v>930</v>
@@ -13070,10 +13064,10 @@
         <v>969</v>
       </c>
       <c r="F201" s="3" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="G201" s="3" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="H201" s="3" t="s">
         <v>946</v>
@@ -13082,7 +13076,7 @@
         <v>930</v>
       </c>
       <c r="K201" s="3" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="L201" s="3" t="s">
         <v>930</v>
@@ -13099,7 +13093,7 @@
         <v>843</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>1419</v>
@@ -13134,10 +13128,10 @@
         <v>844</v>
       </c>
       <c r="C203" s="3" t="s">
+        <v>1647</v>
+      </c>
+      <c r="D203" s="3" t="s">
         <v>1648</v>
-      </c>
-      <c r="D203" s="3" t="s">
-        <v>1649</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>1267</v>
@@ -13528,7 +13522,7 @@
         <v>969</v>
       </c>
       <c r="F214" t="s">
-        <v>1809</v>
+        <v>1806</v>
       </c>
       <c r="G214" t="s">
         <v>1160</v>
@@ -14333,7 +14327,7 @@
         <v>940</v>
       </c>
       <c r="F237" s="3" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="G237" s="3" t="s">
         <v>930</v>
@@ -14368,7 +14362,7 @@
         <v>940</v>
       </c>
       <c r="F238" s="3" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="G238" s="3" t="s">
         <v>1216</v>
@@ -14403,7 +14397,7 @@
         <v>940</v>
       </c>
       <c r="F239" s="3" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="G239" s="3" t="s">
         <v>1216</v>
@@ -14429,10 +14423,10 @@
         <v>108</v>
       </c>
       <c r="C240" s="3" t="s">
+        <v>1649</v>
+      </c>
+      <c r="D240" s="3" t="s">
         <v>1650</v>
-      </c>
-      <c r="D240" s="3" t="s">
-        <v>1651</v>
       </c>
       <c r="E240" s="3" t="s">
         <v>993</v>
@@ -14444,7 +14438,7 @@
         <v>1408</v>
       </c>
       <c r="H240" s="3" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="I240" s="3" t="s">
         <v>930</v>
@@ -14510,7 +14504,7 @@
         <v>967</v>
       </c>
       <c r="F242" s="3" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="G242" s="3" t="s">
         <v>1408</v>
@@ -14539,7 +14533,7 @@
         <v>1249</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>1777</v>
+        <v>1775</v>
       </c>
       <c r="E243" s="3" t="s">
         <v>1044</v>
@@ -14650,7 +14644,7 @@
         <v>969</v>
       </c>
       <c r="F246" s="3" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="G246" s="3" t="s">
         <v>930</v>
@@ -14685,7 +14679,7 @@
         <v>940</v>
       </c>
       <c r="F247" s="3" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="G247" s="3" t="s">
         <v>930</v>
@@ -15047,7 +15041,7 @@
         <v>1404</v>
       </c>
       <c r="K257" s="3" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="L257" s="3" t="s">
         <v>109</v>
@@ -15283,7 +15277,7 @@
         <v>1015</v>
       </c>
       <c r="F264" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="G264" t="s">
         <v>957</v>
@@ -15423,7 +15417,7 @@
         <v>940</v>
       </c>
       <c r="F268" t="s">
-        <v>1821</v>
+        <v>1818</v>
       </c>
       <c r="G268" t="s">
         <v>930</v>
@@ -15458,10 +15452,10 @@
         <v>967</v>
       </c>
       <c r="F269" t="s">
-        <v>1817</v>
+        <v>1814</v>
       </c>
       <c r="G269" t="s">
-        <v>1798</v>
+        <v>1795</v>
       </c>
       <c r="H269" t="s">
         <v>1192</v>
@@ -15522,7 +15516,7 @@
         <v>1359</v>
       </c>
       <c r="D271" t="s">
-        <v>1771</v>
+        <v>1769</v>
       </c>
       <c r="E271" t="s">
         <v>969</v>
@@ -15703,7 +15697,7 @@
         <v>940</v>
       </c>
       <c r="F276" t="s">
-        <v>1818</v>
+        <v>1815</v>
       </c>
       <c r="G276" t="s">
         <v>930</v>
@@ -15729,7 +15723,7 @@
         <v>429</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="D277" s="3" t="s">
         <v>1397</v>
@@ -15753,7 +15747,7 @@
         <v>1404</v>
       </c>
       <c r="K277" s="3" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="L277" s="3" t="s">
         <v>930</v>
@@ -16343,7 +16337,7 @@
         <v>940</v>
       </c>
       <c r="F294" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="G294" t="s">
         <v>1214</v>
@@ -16964,10 +16958,10 @@
         <v>147</v>
       </c>
       <c r="C312" s="3" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="D312" s="6" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="E312" s="3" t="s">
         <v>993</v>
@@ -16979,7 +16973,7 @@
         <v>1490</v>
       </c>
       <c r="H312" s="3" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="L312" s="3" t="s">
         <v>930</v>
@@ -17008,13 +17002,13 @@
         <v>974</v>
       </c>
       <c r="G313" s="3" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="H313" s="3" t="s">
         <v>946</v>
       </c>
       <c r="K313" s="3" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="L313" s="3" t="s">
         <v>930</v>
@@ -17031,10 +17025,10 @@
         <v>378</v>
       </c>
       <c r="C314" s="3" t="s">
+        <v>1663</v>
+      </c>
+      <c r="D314" s="6" t="s">
         <v>1664</v>
-      </c>
-      <c r="D314" s="6" t="s">
-        <v>1665</v>
       </c>
       <c r="E314" s="3" t="s">
         <v>993</v>
@@ -17209,7 +17203,7 @@
         <v>1361</v>
       </c>
       <c r="D319" s="6" t="s">
-        <v>1778</v>
+        <v>1776</v>
       </c>
       <c r="E319" t="s">
         <v>967</v>
@@ -17384,7 +17378,7 @@
         <v>940</v>
       </c>
       <c r="F324" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="G324" t="s">
         <v>1216</v>
@@ -17419,7 +17413,7 @@
         <v>940</v>
       </c>
       <c r="F325" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="G325" t="s">
         <v>1216</v>
@@ -17454,7 +17448,7 @@
         <v>940</v>
       </c>
       <c r="F326" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="G326" t="s">
         <v>1216</v>
@@ -17489,7 +17483,7 @@
         <v>1015</v>
       </c>
       <c r="F327" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="G327" t="s">
         <v>1216</v>
@@ -17909,7 +17903,7 @@
         <v>969</v>
       </c>
       <c r="F339" t="s">
-        <v>1822</v>
+        <v>1819</v>
       </c>
       <c r="G339" t="s">
         <v>1408</v>
@@ -17979,7 +17973,7 @@
         <v>967</v>
       </c>
       <c r="F341" t="s">
-        <v>1814</v>
+        <v>1811</v>
       </c>
       <c r="H341" t="s">
         <v>1241</v>
@@ -18081,7 +18075,7 @@
         <v>940</v>
       </c>
       <c r="F344" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="G344" t="s">
         <v>930</v>
@@ -18641,7 +18635,7 @@
         <v>1255</v>
       </c>
       <c r="D360" t="s">
-        <v>1779</v>
+        <v>1777</v>
       </c>
       <c r="E360" t="s">
         <v>969</v>
@@ -19032,7 +19026,7 @@
         <v>940</v>
       </c>
       <c r="F371" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="G371" t="s">
         <v>930</v>
@@ -19067,7 +19061,7 @@
         <v>940</v>
       </c>
       <c r="F372" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="G372" t="s">
         <v>930</v>
@@ -19102,7 +19096,7 @@
         <v>940</v>
       </c>
       <c r="F373" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="G373" t="s">
         <v>930</v>
@@ -19807,7 +19801,7 @@
         <v>1097</v>
       </c>
       <c r="G393" t="s">
-        <v>1800</v>
+        <v>1797</v>
       </c>
       <c r="H393" t="s">
         <v>930</v>
@@ -20154,7 +20148,7 @@
         <v>940</v>
       </c>
       <c r="F403" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="G403" t="s">
         <v>930</v>
@@ -20183,10 +20177,10 @@
         <v>380</v>
       </c>
       <c r="D404" s="7" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="E404" s="7" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="L404" s="7" t="s">
         <v>930</v>
@@ -20212,7 +20206,7 @@
         <v>940</v>
       </c>
       <c r="F405" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="G405" t="s">
         <v>930</v>
@@ -20247,7 +20241,7 @@
         <v>940</v>
       </c>
       <c r="F406" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="G406" t="s">
         <v>930</v>
@@ -20364,7 +20358,7 @@
         <v>1404</v>
       </c>
       <c r="K409" s="3" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="L409" s="3" t="s">
         <v>806</v>
@@ -20460,7 +20454,7 @@
         <v>940</v>
       </c>
       <c r="F412" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
       <c r="G412" t="s">
         <v>930</v>
@@ -21364,7 +21358,7 @@
         <v>1364</v>
       </c>
       <c r="D438" t="s">
-        <v>1775</v>
+        <v>1773</v>
       </c>
       <c r="E438" t="s">
         <v>1307</v>
@@ -21434,7 +21428,7 @@
         <v>1201</v>
       </c>
       <c r="D440" t="s">
-        <v>1791</v>
+        <v>1789</v>
       </c>
       <c r="E440" t="s">
         <v>1044</v>
@@ -21679,7 +21673,7 @@
         <v>1300</v>
       </c>
       <c r="D447" t="s">
-        <v>1783</v>
+        <v>1781</v>
       </c>
       <c r="E447" t="s">
         <v>1301</v>
@@ -21790,7 +21784,7 @@
         <v>940</v>
       </c>
       <c r="F450" t="s">
-        <v>1800</v>
+        <v>1797</v>
       </c>
       <c r="G450" t="s">
         <v>930</v>
@@ -21860,7 +21854,7 @@
         <v>969</v>
       </c>
       <c r="F452" s="3" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="G452" s="3" t="s">
         <v>1219</v>
@@ -21872,7 +21866,7 @@
         <v>930</v>
       </c>
       <c r="L452" s="3" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="M452" s="3" t="s">
         <v>936</v>
@@ -22665,10 +22659,10 @@
         <v>380</v>
       </c>
       <c r="D475" s="8" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="E475" s="8" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="L475" s="8" t="s">
         <v>930</v>
@@ -23059,7 +23053,7 @@
         <v>1404</v>
       </c>
       <c r="K486" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="L486" t="s">
         <v>1326</v>
@@ -23423,28 +23417,28 @@
         <v>874</v>
       </c>
       <c r="C497" s="3" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="D497" s="3" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="E497" s="3" t="s">
         <v>1015</v>
       </c>
       <c r="F497" s="3" t="s">
+        <v>1672</v>
+      </c>
+      <c r="G497" s="3" t="s">
+        <v>930</v>
+      </c>
+      <c r="H497" s="3" t="s">
         <v>1673</v>
       </c>
-      <c r="G497" s="3" t="s">
-        <v>930</v>
-      </c>
-      <c r="H497" s="3" t="s">
+      <c r="I497" s="3" t="s">
+        <v>930</v>
+      </c>
+      <c r="K497" s="3" t="s">
         <v>1674</v>
-      </c>
-      <c r="I497" s="3" t="s">
-        <v>930</v>
-      </c>
-      <c r="K497" s="3" t="s">
-        <v>1675</v>
       </c>
       <c r="L497" s="3" t="s">
         <v>930</v>
@@ -23499,7 +23493,7 @@
         <v>76</v>
       </c>
       <c r="D499" t="s">
-        <v>1780</v>
+        <v>1778</v>
       </c>
       <c r="E499" t="s">
         <v>1015</v>
@@ -23555,7 +23549,7 @@
         <v>1404</v>
       </c>
       <c r="K500" s="3" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="L500" s="3" t="s">
         <v>930</v>
@@ -23619,7 +23613,7 @@
         <v>930</v>
       </c>
       <c r="G502" s="9" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="H502" s="9" t="s">
         <v>930</v>
@@ -23715,7 +23709,7 @@
         <v>1439</v>
       </c>
       <c r="D505" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
       <c r="E505" t="s">
         <v>967</v>
@@ -23750,7 +23744,7 @@
         <v>1410</v>
       </c>
       <c r="D506" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
       <c r="E506" t="s">
         <v>967</v>
@@ -23782,10 +23776,10 @@
         <v>377</v>
       </c>
       <c r="C507" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="D507" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
       <c r="E507" t="s">
         <v>967</v>
@@ -23852,10 +23846,10 @@
         <v>21</v>
       </c>
       <c r="C509" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="D509" t="s">
-        <v>1769</v>
+        <v>1767</v>
       </c>
       <c r="E509" t="s">
         <v>967</v>
@@ -24091,7 +24085,7 @@
         <v>25794144</v>
       </c>
       <c r="B516" s="11" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="C516" s="11" t="s">
         <v>1348</v>
@@ -24129,10 +24123,10 @@
         <v>46</v>
       </c>
       <c r="C517" s="10" t="s">
+        <v>1678</v>
+      </c>
+      <c r="D517" s="10" t="s">
         <v>1679</v>
-      </c>
-      <c r="D517" s="10" t="s">
-        <v>1680</v>
       </c>
       <c r="E517" s="10" t="s">
         <v>967</v>
@@ -24144,7 +24138,7 @@
         <v>1413</v>
       </c>
       <c r="H517" s="10" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="L517" s="10" t="s">
         <v>930</v>
@@ -24196,19 +24190,19 @@
         <v>320</v>
       </c>
       <c r="C519" s="3" t="s">
+        <v>1681</v>
+      </c>
+      <c r="D519" s="3" t="s">
         <v>1682</v>
-      </c>
-      <c r="D519" s="3" t="s">
-        <v>1683</v>
       </c>
       <c r="E519" s="3" t="s">
         <v>1044</v>
       </c>
       <c r="F519" s="3" t="s">
+        <v>1683</v>
+      </c>
+      <c r="G519" s="3" t="s">
         <v>1684</v>
-      </c>
-      <c r="G519" s="3" t="s">
-        <v>1685</v>
       </c>
       <c r="L519" s="3" t="s">
         <v>109</v>
@@ -24225,7 +24219,7 @@
         <v>118</v>
       </c>
       <c r="C520" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="D520" t="s">
         <v>1419</v>
@@ -24553,7 +24547,7 @@
         <v>1389</v>
       </c>
       <c r="G529" s="3" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
       <c r="H529" s="3" t="s">
         <v>930</v>
@@ -24926,19 +24920,19 @@
         <v>879</v>
       </c>
       <c r="C540" s="3" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="D540" s="3" t="s">
-        <v>1767</v>
+        <v>1765</v>
       </c>
       <c r="E540" s="3" t="s">
         <v>1301</v>
       </c>
       <c r="F540" s="3" t="s">
+        <v>1686</v>
+      </c>
+      <c r="G540" s="3" t="s">
         <v>1687</v>
-      </c>
-      <c r="G540" s="3" t="s">
-        <v>1688</v>
       </c>
       <c r="H540" s="3" t="s">
         <v>930</v>
@@ -25332,7 +25326,7 @@
         <v>930</v>
       </c>
       <c r="H551" s="3" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="I551" s="3" t="s">
         <v>930</v>
@@ -25341,7 +25335,7 @@
         <v>1404</v>
       </c>
       <c r="K551" s="3" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="L551" s="3" t="s">
         <v>930</v>
@@ -25393,10 +25387,10 @@
         <v>880</v>
       </c>
       <c r="C553" s="3" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="D553" s="3" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="E553" s="3" t="s">
         <v>993</v>
@@ -25428,10 +25422,10 @@
         <v>881</v>
       </c>
       <c r="C554" s="3" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="D554" s="3" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="E554" s="3" t="s">
         <v>1236</v>
@@ -25449,7 +25443,7 @@
         <v>930</v>
       </c>
       <c r="K554" s="3" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="L554" s="3" t="s">
         <v>930</v>
@@ -25466,13 +25460,13 @@
         <v>882</v>
       </c>
       <c r="C555" s="3" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="D555" s="3" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="E555" s="3" t="s">
-        <v>1796</v>
+        <v>1793</v>
       </c>
       <c r="F555" s="3" t="s">
         <v>1389</v>
@@ -25487,7 +25481,7 @@
         <v>930</v>
       </c>
       <c r="K555" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="L555" s="3" t="s">
         <v>928</v>
@@ -25504,10 +25498,10 @@
         <v>883</v>
       </c>
       <c r="C556" s="3" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="D556" s="3" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="E556" s="3" t="s">
         <v>967</v>
@@ -25516,10 +25510,10 @@
         <v>1187</v>
       </c>
       <c r="G556" s="3" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="H556" s="3" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="I556" s="3" t="s">
         <v>930</v>
@@ -25539,10 +25533,10 @@
         <v>884</v>
       </c>
       <c r="C557" s="3" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="D557" s="3" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="E557" s="3" t="s">
         <v>993</v>
@@ -25554,7 +25548,7 @@
         <v>1457</v>
       </c>
       <c r="H557" s="3" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="I557" s="3" t="s">
         <v>930</v>
@@ -25574,10 +25568,10 @@
         <v>885</v>
       </c>
       <c r="C558" s="3" t="s">
+        <v>1701</v>
+      </c>
+      <c r="D558" s="3" t="s">
         <v>1702</v>
-      </c>
-      <c r="D558" s="3" t="s">
-        <v>1703</v>
       </c>
       <c r="E558" s="3" t="s">
         <v>1307</v>
@@ -25589,7 +25583,7 @@
         <v>1413</v>
       </c>
       <c r="H558" s="3" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="I558" s="3" t="s">
         <v>930</v>
@@ -25723,7 +25717,7 @@
         <v>940</v>
       </c>
       <c r="F562" t="s">
-        <v>1819</v>
+        <v>1816</v>
       </c>
       <c r="G562" t="s">
         <v>957</v>
@@ -25781,10 +25775,10 @@
         <v>26160542</v>
       </c>
       <c r="B564" s="11" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C564" s="11" t="s">
         <v>1725</v>
-      </c>
-      <c r="C564" s="11" t="s">
-        <v>1726</v>
       </c>
       <c r="D564" s="11" t="s">
         <v>1553</v>
@@ -25886,7 +25880,7 @@
         <v>26166496</v>
       </c>
       <c r="B567" s="11" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="C567" s="11" t="s">
         <v>822</v>
@@ -25901,7 +25895,7 @@
         <v>930</v>
       </c>
       <c r="G567" s="11" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="H567" s="11" t="s">
         <v>1534</v>
@@ -26400,13 +26394,13 @@
         <v>1043</v>
       </c>
       <c r="D581" s="3" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="E581" s="3" t="s">
         <v>1489</v>
       </c>
       <c r="F581" s="3" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="G581" s="3" t="s">
         <v>1071</v>
@@ -26476,7 +26470,7 @@
         <v>940</v>
       </c>
       <c r="F583" s="3" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="G583" s="3" t="s">
         <v>930</v>
@@ -26902,7 +26896,7 @@
         <v>1459</v>
       </c>
       <c r="D595" t="s">
-        <v>1774</v>
+        <v>1772</v>
       </c>
       <c r="E595" s="3" t="s">
         <v>993</v>
@@ -26978,7 +26972,7 @@
         <v>1462</v>
       </c>
       <c r="D597" t="s">
-        <v>1786</v>
+        <v>1784</v>
       </c>
       <c r="E597" s="3" t="s">
         <v>993</v>
@@ -27013,7 +27007,7 @@
         <v>1463</v>
       </c>
       <c r="D598" t="s">
-        <v>1763</v>
+        <v>1761</v>
       </c>
       <c r="E598" s="3" t="s">
         <v>1267</v>
@@ -27048,7 +27042,7 @@
         <v>1464</v>
       </c>
       <c r="D599" t="s">
-        <v>1792</v>
+        <v>1790</v>
       </c>
       <c r="E599" s="3" t="s">
         <v>993</v>
@@ -27258,7 +27252,7 @@
         <v>1249</v>
       </c>
       <c r="D605" t="s">
-        <v>1788</v>
+        <v>1786</v>
       </c>
       <c r="E605" s="3" t="s">
         <v>967</v>
@@ -27322,7 +27316,7 @@
         <v>355</v>
       </c>
       <c r="C607" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="D607" t="s">
         <v>1473</v>
@@ -27614,7 +27608,7 @@
         <v>1015</v>
       </c>
       <c r="F615" s="3" t="s">
-        <v>1804</v>
+        <v>1801</v>
       </c>
       <c r="G615" s="3" t="s">
         <v>930</v>
@@ -27885,7 +27879,7 @@
         <v>125</v>
       </c>
       <c r="C623" t="s">
-        <v>1758</v>
+        <v>1756</v>
       </c>
       <c r="D623" t="s">
         <v>1481</v>
@@ -28034,7 +28028,7 @@
         <v>1043</v>
       </c>
       <c r="D627" t="s">
-        <v>1781</v>
+        <v>1779</v>
       </c>
       <c r="E627" s="3" t="s">
         <v>967</v>
@@ -28174,7 +28168,7 @@
         <v>104</v>
       </c>
       <c r="C631" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="D631" t="s">
         <v>1484</v>
@@ -28364,7 +28358,7 @@
         <v>969</v>
       </c>
       <c r="F636" s="3" t="s">
-        <v>1814</v>
+        <v>1811</v>
       </c>
       <c r="H636" s="3" t="s">
         <v>1013</v>
@@ -28495,7 +28489,7 @@
         <v>1488</v>
       </c>
       <c r="D640" t="s">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="E640" s="3" t="s">
         <v>1489</v>
@@ -29980,7 +29974,7 @@
         <v>694</v>
       </c>
       <c r="C682" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="D682" t="s">
         <v>1509</v>
@@ -29992,7 +29986,7 @@
         <v>986</v>
       </c>
       <c r="G682" s="3" t="s">
-        <v>1802</v>
+        <v>1799</v>
       </c>
       <c r="H682" s="3" t="s">
         <v>930</v>
@@ -30129,7 +30123,7 @@
         <v>888</v>
       </c>
       <c r="C686" s="3" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="D686" s="3" t="s">
         <v>1335</v>
@@ -30153,7 +30147,7 @@
         <v>1406</v>
       </c>
       <c r="K686" s="3" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="L686" s="3" t="s">
         <v>930</v>
@@ -30593,7 +30587,7 @@
         <v>701</v>
       </c>
       <c r="C699" t="s">
-        <v>1750</v>
+        <v>1822</v>
       </c>
       <c r="D699" t="s">
         <v>1518</v>
@@ -30628,10 +30622,10 @@
         <v>702</v>
       </c>
       <c r="C700" t="s">
-        <v>1794</v>
+        <v>1791</v>
       </c>
       <c r="D700" t="s">
-        <v>1795</v>
+        <v>1792</v>
       </c>
       <c r="E700" t="s">
         <v>967</v>
@@ -31013,7 +31007,7 @@
         <v>709</v>
       </c>
       <c r="C711" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="D711" t="s">
         <v>930</v>
@@ -31022,7 +31016,7 @@
         <v>967</v>
       </c>
       <c r="F711" s="3" t="s">
-        <v>1805</v>
+        <v>1802</v>
       </c>
       <c r="G711" s="3" t="s">
         <v>930</v>
@@ -31410,7 +31404,7 @@
         <v>940</v>
       </c>
       <c r="F722" s="3" t="s">
-        <v>1797</v>
+        <v>1794</v>
       </c>
       <c r="G722" s="3" t="s">
         <v>930</v>
@@ -31573,7 +31567,7 @@
         <v>27536294</v>
       </c>
       <c r="B727" s="5" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="C727" s="5" t="s">
         <v>76</v>
@@ -31696,7 +31690,7 @@
         <v>969</v>
       </c>
       <c r="F730" s="3" t="s">
-        <v>1810</v>
+        <v>1807</v>
       </c>
       <c r="G730" s="3" t="s">
         <v>930</v>
@@ -31731,7 +31725,7 @@
         <v>969</v>
       </c>
       <c r="F731" s="3" t="s">
-        <v>1820</v>
+        <v>1817</v>
       </c>
       <c r="G731" s="3" t="s">
         <v>930</v>
@@ -31836,7 +31830,7 @@
         <v>1201</v>
       </c>
       <c r="D734" t="s">
-        <v>1770</v>
+        <v>1768</v>
       </c>
       <c r="E734" t="s">
         <v>967</v>
@@ -31900,7 +31894,7 @@
         <v>727</v>
       </c>
       <c r="C736" t="s">
-        <v>1511</v>
+        <v>45</v>
       </c>
       <c r="D736" t="s">
         <v>790</v>
@@ -32323,7 +32317,7 @@
         <v>1539</v>
       </c>
       <c r="D748" t="s">
-        <v>1765</v>
+        <v>1763</v>
       </c>
       <c r="E748" t="s">
         <v>1489</v>
@@ -32390,10 +32384,10 @@
         <v>732</v>
       </c>
       <c r="C750" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="D750" t="s">
-        <v>1766</v>
+        <v>1764</v>
       </c>
       <c r="E750" t="s">
         <v>1542</v>
@@ -32600,7 +32594,7 @@
         <v>738</v>
       </c>
       <c r="C756" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="D756" t="s">
         <v>1548</v>
@@ -32746,7 +32740,7 @@
         <v>742</v>
       </c>
       <c r="C760" t="s">
-        <v>1757</v>
+        <v>1755</v>
       </c>
       <c r="D760" t="s">
         <v>1397</v>
@@ -32928,7 +32922,7 @@
         <v>747</v>
       </c>
       <c r="C765" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="D765" t="s">
         <v>1419</v>
@@ -33745,10 +33739,10 @@
         <v>891</v>
       </c>
       <c r="C788" t="s">
-        <v>1751</v>
+        <v>1749</v>
       </c>
       <c r="D788" t="s">
-        <v>1768</v>
+        <v>1766</v>
       </c>
       <c r="E788" t="s">
         <v>967</v>
@@ -34101,7 +34095,7 @@
         <v>1573</v>
       </c>
       <c r="D798" t="s">
-        <v>1793</v>
+        <v>1116</v>
       </c>
       <c r="E798" t="s">
         <v>969</v>
@@ -34203,10 +34197,10 @@
         <v>904</v>
       </c>
       <c r="C801" t="s">
-        <v>1754</v>
+        <v>1752</v>
       </c>
       <c r="D801" t="s">
-        <v>1753</v>
+        <v>1751</v>
       </c>
       <c r="E801" t="s">
         <v>967</v>
@@ -34238,10 +34232,10 @@
         <v>905</v>
       </c>
       <c r="C802" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="D802" t="s">
-        <v>1755</v>
+        <v>1753</v>
       </c>
       <c r="E802" t="s">
         <v>967</v>
@@ -34448,16 +34442,16 @@
         <v>911</v>
       </c>
       <c r="C808" s="3" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D808" s="3" t="s">
-        <v>1772</v>
+        <v>1770</v>
       </c>
       <c r="E808" s="3" t="s">
         <v>967</v>
       </c>
       <c r="F808" s="3" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="G808" s="3" t="s">
         <v>1219</v>
@@ -34483,10 +34477,10 @@
         <v>912</v>
       </c>
       <c r="C809" s="3" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D809" s="3" t="s">
-        <v>1773</v>
+        <v>1771</v>
       </c>
       <c r="E809" s="3" t="s">
         <v>967</v>
@@ -34504,7 +34498,7 @@
         <v>930</v>
       </c>
       <c r="K809" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="L809" s="3" t="s">
         <v>930</v>
@@ -34542,7 +34536,7 @@
         <v>930</v>
       </c>
       <c r="K810" s="10" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="L810" s="10" t="s">
         <v>930</v>
@@ -34594,7 +34588,7 @@
         <v>915</v>
       </c>
       <c r="C812" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="D812" t="s">
         <v>1581</v>
@@ -34667,7 +34661,7 @@
         <v>1585</v>
       </c>
       <c r="D814" t="s">
-        <v>1763</v>
+        <v>1761</v>
       </c>
       <c r="E814" t="s">
         <v>993</v>
@@ -34702,7 +34696,7 @@
         <v>1586</v>
       </c>
       <c r="D815" t="s">
-        <v>1790</v>
+        <v>1788</v>
       </c>
       <c r="E815" t="s">
         <v>1236</v>
@@ -34734,7 +34728,7 @@
         <v>919</v>
       </c>
       <c r="C816" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="D816" t="s">
         <v>1572</v>
@@ -35014,16 +35008,16 @@
         <v>763</v>
       </c>
       <c r="C824" s="3" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="D824" s="3" t="s">
-        <v>1782</v>
+        <v>1780</v>
       </c>
       <c r="E824" s="3" t="s">
         <v>969</v>
       </c>
       <c r="F824" s="3" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="G824" s="3" t="s">
         <v>930</v>
@@ -35049,10 +35043,10 @@
         <v>764</v>
       </c>
       <c r="C825" s="3" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="D825" s="3" t="s">
-        <v>1784</v>
+        <v>1782</v>
       </c>
       <c r="E825" s="3" t="s">
         <v>1303</v>
@@ -35087,7 +35081,7 @@
         <v>1596</v>
       </c>
       <c r="D826" t="s">
-        <v>1789</v>
+        <v>1787</v>
       </c>
       <c r="E826" t="s">
         <v>967</v>
@@ -35233,7 +35227,7 @@
         <v>940</v>
       </c>
       <c r="F830" s="3" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="G830" s="3" t="s">
         <v>930</v>
@@ -35659,7 +35653,7 @@
         <v>967</v>
       </c>
       <c r="F842" t="s">
-        <v>1806</v>
+        <v>1803</v>
       </c>
       <c r="G842" t="s">
         <v>930</v>
@@ -35717,7 +35711,7 @@
         <v>28642469</v>
       </c>
       <c r="B844" s="3" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="C844" s="3" t="s">
         <v>154</v>
@@ -35980,7 +35974,7 @@
         <v>1607</v>
       </c>
       <c r="G851" t="s">
-        <v>1803</v>
+        <v>1800</v>
       </c>
       <c r="H851" t="s">
         <v>930</v>
@@ -36003,7 +35997,7 @@
         <v>781</v>
       </c>
       <c r="C852" t="s">
-        <v>1752</v>
+        <v>1750</v>
       </c>
       <c r="D852" t="s">
         <v>1529</v>

</xml_diff>

<commit_message>
appearance + minor errors
</commit_message>
<xml_diff>
--- a/data/figure_classification_final.xlsx
+++ b/data/figure_classification_final.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acrisan/Projects/gevit_gallery_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3B3E04EB-9D99-5949-978A-681D88F1935B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0E42316F-2597-5141-818A-4465CDFDFECD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="figure_classification_final" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">figure_classification_final!$A$1:$M$856</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -6311,11 +6314,14 @@
   <dimension ref="A1:M856"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J126" sqref="J126"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="40" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>